<commit_message>
På vej til transformation
</commit_message>
<xml_diff>
--- a/results/Gaia_homogeneous_target_selection_M_earth_1.5_Jinglin_2025.01.09.xlsx
+++ b/results/Gaia_homogeneous_target_selection_M_earth_1.5_Jinglin_2025.01.09.xlsx
@@ -474,7 +474,7 @@
     <col width="13" customWidth="1" min="25" max="25"/>
     <col width="26" customWidth="1" min="26" max="26"/>
     <col width="22" customWidth="1" min="27" max="27"/>
-    <col width="39" customWidth="1" min="28" max="28"/>
+    <col width="24" customWidth="1" min="28" max="28"/>
     <col width="41" customWidth="1" min="29" max="29"/>
     <col width="19" customWidth="1" min="30" max="30"/>
     <col width="13" customWidth="1" min="31" max="31"/>
@@ -618,7 +618,7 @@
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Readable Spectral Type (experimental)</t>
+          <t>Readable Spectral Type</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
@@ -734,16 +734,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
       <c r="AC2" t="n">
         <v>0.2915670197316235</v>
       </c>
@@ -864,7 +854,7 @@
         <v>0.3573652612687087</v>
       </c>
       <c r="AD3" t="n">
-        <v>3.652170961142576</v>
+        <v>3.652170961142577</v>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
@@ -928,10 +918,10 @@
         <v>0.6801935396018817</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.04760277646490328</v>
+        <v>0.04760277646490326</v>
       </c>
       <c r="R4" t="n">
-        <v>0.3846692630478291</v>
+        <v>0.3846692630478289</v>
       </c>
       <c r="S4" t="n">
         <v>2.216291768419251</v>
@@ -969,18 +959,8 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>K5V</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>K5V</t>
-        </is>
-      </c>
       <c r="AC4" t="n">
-        <v>0.3846689737009667</v>
+        <v>0.3846689737009666</v>
       </c>
       <c r="AD4" t="n">
         <v>3.638438981826665</v>
@@ -1078,16 +1058,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>K0V</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>K0V</t>
-        </is>
-      </c>
       <c r="AC5" t="n">
         <v>0.4450389844451547</v>
       </c>
@@ -1194,16 +1164,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>K0V</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>K0V</t>
-        </is>
-      </c>
       <c r="AC6" t="n">
         <v>0.4771345237448785</v>
       </c>
@@ -1313,16 +1273,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>G6V</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>G6V</t>
-        </is>
-      </c>
       <c r="AC7" t="n">
         <v>0.5142611276059875</v>
       </c>
@@ -1432,16 +1382,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>G8IV</t>
-        </is>
-      </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>G8IV</t>
-        </is>
-      </c>
       <c r="AC8" t="n">
         <v>0.5223206596684706</v>
       </c>
@@ -1546,21 +1486,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
-      <c r="AB9" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
       <c r="AC9" t="n">
         <v>0.5290407979530127</v>
       </c>
       <c r="AD9" t="n">
-        <v>5.952271867918356</v>
+        <v>5.952271867918357</v>
       </c>
       <c r="AE9" t="inlineStr">
         <is>
@@ -1660,21 +1590,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA10" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
-      <c r="AB10" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
       <c r="AC10" t="n">
         <v>0.5294743225641715</v>
       </c>
       <c r="AD10" t="n">
-        <v>5.947768672408886</v>
+        <v>5.947768672408884</v>
       </c>
       <c r="AE10" t="inlineStr">
         <is>
@@ -1771,16 +1691,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA11" t="inlineStr">
-        <is>
-          <t>K2.5V</t>
-        </is>
-      </c>
-      <c r="AB11" t="inlineStr">
-        <is>
-          <t>K2.5V</t>
-        </is>
-      </c>
       <c r="AC11" t="n">
         <v>0.5590275095562457</v>
       </c>
@@ -1896,7 +1806,7 @@
         <v>0.5730966165167038</v>
       </c>
       <c r="AD12" t="n">
-        <v>7.478346136538076</v>
+        <v>7.478346136538074</v>
       </c>
     </row>
     <row r="13">
@@ -1991,21 +1901,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA13" t="inlineStr">
-        <is>
-          <t>G7Ve</t>
-        </is>
-      </c>
-      <c r="AB13" t="inlineStr">
-        <is>
-          <t>G7V</t>
-        </is>
-      </c>
       <c r="AC13" t="n">
         <v>0.5942699633082099</v>
       </c>
       <c r="AD13" t="n">
-        <v>6.753585334578519</v>
+        <v>6.753585334578522</v>
       </c>
       <c r="AE13" t="inlineStr">
         <is>
@@ -2229,16 +2129,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA15" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
-      <c r="AB15" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
       <c r="AC15" t="n">
         <v>0.6633463321963884</v>
       </c>
@@ -2348,21 +2238,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA16" t="inlineStr">
-        <is>
-          <t>K2.5V</t>
-        </is>
-      </c>
-      <c r="AB16" t="inlineStr">
-        <is>
-          <t>K2.5V</t>
-        </is>
-      </c>
       <c r="AC16" t="n">
         <v>0.6932365286912114</v>
       </c>
       <c r="AD16" t="n">
-        <v>7.435229060298578</v>
+        <v>7.435229060298576</v>
       </c>
       <c r="AE16" t="inlineStr">
         <is>
@@ -2423,7 +2303,7 @@
         <v>0.79312927</v>
       </c>
       <c r="P17" t="n">
-        <v>0.7729086508056566</v>
+        <v>0.7729086508056565</v>
       </c>
       <c r="Q17" t="n">
         <v>0.08059422994419436</v>
@@ -2459,21 +2339,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA17" t="inlineStr">
-        <is>
-          <t>K3V</t>
-        </is>
-      </c>
-      <c r="AB17" t="inlineStr">
-        <is>
-          <t>K3V</t>
-        </is>
-      </c>
       <c r="AC17" t="n">
         <v>0.7087923524028937</v>
       </c>
       <c r="AD17" t="n">
-        <v>7.228567098899185</v>
+        <v>7.228567098899183</v>
       </c>
       <c r="AE17" t="inlineStr">
         <is>
@@ -2578,16 +2448,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA18" t="inlineStr">
-        <is>
-          <t>K5V</t>
-        </is>
-      </c>
-      <c r="AB18" t="inlineStr">
-        <is>
-          <t>K5V</t>
-        </is>
-      </c>
       <c r="AC18" t="n">
         <v>0.7177597081872569</v>
       </c>
@@ -2697,21 +2557,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA19" t="inlineStr">
-        <is>
-          <t>G9V</t>
-        </is>
-      </c>
-      <c r="AB19" t="inlineStr">
-        <is>
-          <t>G9V</t>
-        </is>
-      </c>
       <c r="AC19" t="n">
         <v>0.7237436201563109</v>
       </c>
       <c r="AD19" t="n">
-        <v>8.791104886960108</v>
+        <v>8.791104886960111</v>
       </c>
       <c r="AE19" t="inlineStr">
         <is>
@@ -2813,16 +2663,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA20" t="inlineStr">
-        <is>
-          <t>G6.5V</t>
-        </is>
-      </c>
-      <c r="AB20" t="inlineStr">
-        <is>
-          <t>G6.5V</t>
-        </is>
-      </c>
       <c r="AC20" t="n">
         <v>0.7300811231546194</v>
       </c>
@@ -2927,16 +2767,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA21" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
-      <c r="AB21" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
       <c r="AC21" t="n">
         <v>0.7544239895301074</v>
       </c>
@@ -3041,21 +2871,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA22" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
-      <c r="AB22" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
       <c r="AC22" t="n">
         <v>0.7580177000040715</v>
       </c>
       <c r="AD22" t="n">
-        <v>8.196488023769632</v>
+        <v>8.196488023769628</v>
       </c>
       <c r="AE22" t="inlineStr">
         <is>
@@ -3152,21 +2972,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA23" t="inlineStr">
-        <is>
-          <t>K4V</t>
-        </is>
-      </c>
-      <c r="AB23" t="inlineStr">
-        <is>
-          <t>K4V</t>
-        </is>
-      </c>
       <c r="AC23" t="n">
         <v>0.7582418672732505</v>
       </c>
       <c r="AD23" t="n">
-        <v>5.105783367734122</v>
+        <v>5.105783367734121</v>
       </c>
       <c r="AE23" t="inlineStr">
         <is>
@@ -3271,21 +3081,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA24" t="inlineStr">
-        <is>
-          <t>K2+V</t>
-        </is>
-      </c>
-      <c r="AB24" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
       <c r="AC24" t="n">
         <v>0.7586321818386983</v>
       </c>
       <c r="AD24" t="n">
-        <v>8.811567976359873</v>
+        <v>8.811567976359871</v>
       </c>
       <c r="AE24" t="inlineStr">
         <is>
@@ -3390,21 +3190,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA25" t="inlineStr">
-        <is>
-          <t>F9.5V</t>
-        </is>
-      </c>
-      <c r="AB25" t="inlineStr">
-        <is>
-          <t>F9.5V</t>
-        </is>
-      </c>
       <c r="AC25" t="n">
         <v>0.7800602061975175</v>
       </c>
       <c r="AD25" t="n">
-        <v>8.607142418062876</v>
+        <v>8.607142418062878</v>
       </c>
       <c r="AE25" t="inlineStr">
         <is>
@@ -3509,21 +3299,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA26" t="inlineStr">
-        <is>
-          <t>G0V</t>
-        </is>
-      </c>
-      <c r="AB26" t="inlineStr">
-        <is>
-          <t>G0V</t>
-        </is>
-      </c>
       <c r="AC26" t="n">
         <v>0.7940756748333149</v>
       </c>
       <c r="AD26" t="n">
-        <v>8.699460211492761</v>
+        <v>8.699460211492765</v>
       </c>
       <c r="AE26" t="inlineStr">
         <is>
@@ -3628,16 +3408,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA27" t="inlineStr">
-        <is>
-          <t>G2V</t>
-        </is>
-      </c>
-      <c r="AB27" t="inlineStr">
-        <is>
-          <t>G2V</t>
-        </is>
-      </c>
       <c r="AC27" t="n">
         <v>0.7950825050741951</v>
       </c>
@@ -3747,21 +3517,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA28" t="inlineStr">
-        <is>
-          <t>F9.5V</t>
-        </is>
-      </c>
-      <c r="AB28" t="inlineStr">
-        <is>
-          <t>F9.5V</t>
-        </is>
-      </c>
       <c r="AC28" t="n">
         <v>0.8258618156774155</v>
       </c>
       <c r="AD28" t="n">
-        <v>9.197515891787265</v>
+        <v>9.197515891787267</v>
       </c>
       <c r="AE28" t="inlineStr">
         <is>
@@ -3866,21 +3626,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA29" t="inlineStr">
-        <is>
-          <t>K4Ve</t>
-        </is>
-      </c>
-      <c r="AB29" t="inlineStr">
-        <is>
-          <t>K4V</t>
-        </is>
-      </c>
       <c r="AC29" t="n">
         <v>0.836636116717227</v>
       </c>
       <c r="AD29" t="n">
-        <v>7.601527372616971</v>
+        <v>7.601527372616974</v>
       </c>
       <c r="AE29" t="inlineStr">
         <is>
@@ -3980,21 +3730,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA30" t="inlineStr">
-        <is>
-          <t>K2.5V(k)</t>
-        </is>
-      </c>
-      <c r="AB30" t="inlineStr">
-        <is>
-          <t>K2.5V</t>
-        </is>
-      </c>
       <c r="AC30" t="n">
         <v>0.8408143061232506</v>
       </c>
       <c r="AD30" t="n">
-        <v>8.891570979811476</v>
+        <v>8.89157097981148</v>
       </c>
       <c r="AE30" t="inlineStr">
         <is>
@@ -4210,21 +3950,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA32" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
-      <c r="AB32" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
       <c r="AC32" t="n">
         <v>0.8427702230441656</v>
       </c>
       <c r="AD32" t="n">
-        <v>9.893947947441868</v>
+        <v>9.893947947441871</v>
       </c>
       <c r="AE32" t="inlineStr">
         <is>
@@ -4448,16 +4178,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA34" t="inlineStr">
-        <is>
-          <t>G7V</t>
-        </is>
-      </c>
-      <c r="AB34" t="inlineStr">
-        <is>
-          <t>G7V</t>
-        </is>
-      </c>
       <c r="AC34" t="n">
         <v>0.8540485482395566</v>
       </c>
@@ -4567,16 +4287,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA35" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
-      <c r="AB35" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
       <c r="AC35" t="n">
         <v>0.864916731614888</v>
       </c>
@@ -4695,7 +4405,7 @@
         <v>0.886454969254667</v>
       </c>
       <c r="AD36" t="n">
-        <v>6.74858017749629</v>
+        <v>6.748580177496287</v>
       </c>
       <c r="AE36" t="inlineStr">
         <is>
@@ -4800,21 +4510,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA37" t="inlineStr">
-        <is>
-          <t>K3.5V</t>
-        </is>
-      </c>
-      <c r="AB37" t="inlineStr">
-        <is>
-          <t>K3.5V</t>
-        </is>
-      </c>
       <c r="AC37" t="n">
         <v>0.9032258933011167</v>
       </c>
       <c r="AD37" t="n">
-        <v>8.744719768346879</v>
+        <v>8.744719768346878</v>
       </c>
       <c r="AE37" t="inlineStr">
         <is>
@@ -4919,16 +4619,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA38" t="inlineStr">
-        <is>
-          <t>F9V</t>
-        </is>
-      </c>
-      <c r="AB38" t="inlineStr">
-        <is>
-          <t>F9V</t>
-        </is>
-      </c>
       <c r="AC38" t="n">
         <v>0.916376850247449</v>
       </c>
@@ -5083,7 +4773,7 @@
         <v>-32.82768460705796</v>
       </c>
       <c r="F40" t="n">
-        <v>5.927006939272881</v>
+        <v>5.92700693927288</v>
       </c>
       <c r="G40" t="n">
         <v>5.73832368850708</v>
@@ -5116,10 +4806,10 @@
         <v>0.8504255555675814</v>
       </c>
       <c r="Q40" t="n">
-        <v>0.09853843814150051</v>
+        <v>0.09853843814150043</v>
       </c>
       <c r="R40" t="n">
-        <v>0.9431872317280452</v>
+        <v>0.9431872317280443</v>
       </c>
       <c r="S40" t="n">
         <v>1.863068063832381</v>
@@ -5157,18 +4847,8 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA40" t="inlineStr">
-        <is>
-          <t>K0V</t>
-        </is>
-      </c>
-      <c r="AB40" t="inlineStr">
-        <is>
-          <t>K0V</t>
-        </is>
-      </c>
       <c r="AC40" t="n">
-        <v>0.9431856815929422</v>
+        <v>0.9431856815929414</v>
       </c>
       <c r="AD40" t="n">
         <v>9.559015075372868</v>
@@ -5276,16 +4956,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA41" t="inlineStr">
-        <is>
-          <t>K0.5V</t>
-        </is>
-      </c>
-      <c r="AB41" t="inlineStr">
-        <is>
-          <t>K0.5V</t>
-        </is>
-      </c>
       <c r="AC41" t="n">
         <v>0.9605020925049499</v>
       </c>
@@ -5387,16 +5057,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA42" t="inlineStr">
-        <is>
-          <t>K3-V</t>
-        </is>
-      </c>
-      <c r="AB42" t="inlineStr">
-        <is>
-          <t>K3V</t>
-        </is>
-      </c>
       <c r="AC42" t="n">
         <v>0.9749778190568295</v>
       </c>
@@ -5498,16 +5158,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA43" t="inlineStr">
-        <is>
-          <t>G0-V</t>
-        </is>
-      </c>
-      <c r="AB43" t="inlineStr">
-        <is>
-          <t>G0V</t>
-        </is>
-      </c>
       <c r="AC43" t="n">
         <v>0.9792103388426828</v>
       </c>
@@ -5617,16 +5267,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA44" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
-      <c r="AB44" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
       <c r="AC44" t="n">
         <v>0.991114835394329</v>
       </c>
@@ -5736,16 +5376,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA45" t="inlineStr">
-        <is>
-          <t>K1.5V</t>
-        </is>
-      </c>
-      <c r="AB45" t="inlineStr">
-        <is>
-          <t>K1.5V</t>
-        </is>
-      </c>
       <c r="AC45" t="n">
         <v>0.9971189887205378</v>
       </c>
@@ -5855,16 +5485,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA46" t="inlineStr">
-        <is>
-          <t>K7+Vk</t>
-        </is>
-      </c>
-      <c r="AB46" t="inlineStr">
-        <is>
-          <t>K7V</t>
-        </is>
-      </c>
       <c r="AC46" t="n">
         <v>1.001676513284205</v>
       </c>
@@ -5985,7 +5605,7 @@
         <v>1.00496033301819</v>
       </c>
       <c r="AD47" t="n">
-        <v>7.713318653486467</v>
+        <v>7.713318653486466</v>
       </c>
       <c r="AE47" t="inlineStr">
         <is>
@@ -6090,16 +5710,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA48" t="inlineStr">
-        <is>
-          <t>K3V</t>
-        </is>
-      </c>
-      <c r="AB48" t="inlineStr">
-        <is>
-          <t>K3V</t>
-        </is>
-      </c>
       <c r="AC48" t="n">
         <v>1.01282488433344</v>
       </c>
@@ -6209,16 +5819,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA49" t="inlineStr">
-        <is>
-          <t>G7IVHdel1</t>
-        </is>
-      </c>
-      <c r="AB49" t="inlineStr">
-        <is>
-          <t>G7IV</t>
-        </is>
-      </c>
       <c r="AC49" t="n">
         <v>1.034562799168904</v>
       </c>
@@ -6328,16 +5928,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA50" t="inlineStr">
-        <is>
-          <t>G8IV</t>
-        </is>
-      </c>
-      <c r="AB50" t="inlineStr">
-        <is>
-          <t>G8IV</t>
-        </is>
-      </c>
       <c r="AC50" t="n">
         <v>1.036210068060923</v>
       </c>
@@ -6447,16 +6037,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA51" t="inlineStr">
-        <is>
-          <t>G8:V</t>
-        </is>
-      </c>
-      <c r="AB51" t="inlineStr">
-        <is>
-          <t>G8</t>
-        </is>
-      </c>
       <c r="AC51" t="n">
         <v>1.057956762473487</v>
       </c>
@@ -6923,16 +6503,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA55" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
-      <c r="AB55" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
       <c r="AC55" t="n">
         <v>1.075774763359316</v>
       </c>
@@ -6996,7 +6566,7 @@
         <v>2.358674017254114</v>
       </c>
       <c r="Q56" t="n">
-        <v>0.05889773285453718</v>
+        <v>0.05889773285453719</v>
       </c>
       <c r="R56" t="n">
         <v>1.081426383332846</v>
@@ -7035,16 +6605,6 @@
       <c r="Z56" t="inlineStr">
         <is>
           <t>GAIA</t>
-        </is>
-      </c>
-      <c r="AA56" t="inlineStr">
-        <is>
-          <t>F9IV-V</t>
-        </is>
-      </c>
-      <c r="AB56" t="inlineStr">
-        <is>
-          <t>F9IV-V</t>
         </is>
       </c>
       <c r="AC56" t="n">
@@ -7156,16 +6716,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA57" t="inlineStr">
-        <is>
-          <t>G1V</t>
-        </is>
-      </c>
-      <c r="AB57" t="inlineStr">
-        <is>
-          <t>G1V</t>
-        </is>
-      </c>
       <c r="AC57" t="n">
         <v>1.114014128811055</v>
       </c>
@@ -7275,16 +6825,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA58" t="inlineStr">
-        <is>
-          <t>G8V</t>
-        </is>
-      </c>
-      <c r="AB58" t="inlineStr">
-        <is>
-          <t>G8V</t>
-        </is>
-      </c>
       <c r="AC58" t="n">
         <v>1.117419989728082</v>
       </c>
@@ -7394,16 +6934,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA59" t="inlineStr">
-        <is>
-          <t>G2.5VHdel1</t>
-        </is>
-      </c>
-      <c r="AB59" t="inlineStr">
-        <is>
-          <t>G2.5V</t>
-        </is>
-      </c>
       <c r="AC59" t="n">
         <v>1.131500929397614</v>
       </c>
@@ -7513,16 +7043,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA60" t="inlineStr">
-        <is>
-          <t>F9V</t>
-        </is>
-      </c>
-      <c r="AB60" t="inlineStr">
-        <is>
-          <t>F9V</t>
-        </is>
-      </c>
       <c r="AC60" t="n">
         <v>1.132885192269361</v>
       </c>
@@ -7632,16 +7152,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA61" t="inlineStr">
-        <is>
-          <t>G3IV-V</t>
-        </is>
-      </c>
-      <c r="AB61" t="inlineStr">
-        <is>
-          <t>G3IV-V</t>
-        </is>
-      </c>
       <c r="AC61" t="n">
         <v>1.13511944648496</v>
       </c>
@@ -7751,16 +7261,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA62" t="inlineStr">
-        <is>
-          <t>G5V</t>
-        </is>
-      </c>
-      <c r="AB62" t="inlineStr">
-        <is>
-          <t>G5V</t>
-        </is>
-      </c>
       <c r="AC62" t="n">
         <v>1.156399616152608</v>
       </c>
@@ -7870,16 +7370,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA63" t="inlineStr">
-        <is>
-          <t>G1V</t>
-        </is>
-      </c>
-      <c r="AB63" t="inlineStr">
-        <is>
-          <t>G1V</t>
-        </is>
-      </c>
       <c r="AC63" t="n">
         <v>1.156892104030787</v>
       </c>
@@ -7989,16 +7479,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA64" t="inlineStr">
-        <is>
-          <t>G8V</t>
-        </is>
-      </c>
-      <c r="AB64" t="inlineStr">
-        <is>
-          <t>G8V</t>
-        </is>
-      </c>
       <c r="AC64" t="n">
         <v>1.162391131437627</v>
       </c>
@@ -8105,16 +7585,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA65" t="inlineStr">
-        <is>
-          <t>K3+V</t>
-        </is>
-      </c>
-      <c r="AB65" t="inlineStr">
-        <is>
-          <t>K3V</t>
-        </is>
-      </c>
       <c r="AC65" t="n">
         <v>1.166829181339082</v>
       </c>
@@ -8224,16 +7694,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA66" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
-      <c r="AB66" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
       <c r="AC66" t="n">
         <v>1.176752583020998</v>
       </c>
@@ -8302,10 +7762,10 @@
         <v>1.333443199020918</v>
       </c>
       <c r="Q67" t="n">
-        <v>0.09325466522786471</v>
+        <v>0.09325466522786466</v>
       </c>
       <c r="R67" t="n">
-        <v>1.183535918713182</v>
+        <v>1.183535918713181</v>
       </c>
       <c r="S67" t="n">
         <v>0.94254112753729</v>
@@ -8343,18 +7803,8 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA67" t="inlineStr">
-        <is>
-          <t>G2.5IV-V</t>
-        </is>
-      </c>
-      <c r="AB67" t="inlineStr">
-        <is>
-          <t>G2.5IV-V</t>
-        </is>
-      </c>
       <c r="AC67" t="n">
-        <v>1.1835337418176</v>
+        <v>1.183533741817599</v>
       </c>
       <c r="AD67" t="n">
         <v>13.23996519741542</v>
@@ -8575,16 +8025,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA69" t="inlineStr">
-        <is>
-          <t>G4Va</t>
-        </is>
-      </c>
-      <c r="AB69" t="inlineStr">
-        <is>
-          <t>G4V</t>
-        </is>
-      </c>
       <c r="AC69" t="n">
         <v>1.1946846420043</v>
       </c>
@@ -8653,10 +8093,10 @@
         <v>1.300233921808833</v>
       </c>
       <c r="Q70" t="n">
-        <v>0.09573618983673104</v>
+        <v>0.09573618983673095</v>
       </c>
       <c r="R70" t="n">
-        <v>1.197932611991165</v>
+        <v>1.197932611991164</v>
       </c>
       <c r="S70" t="n">
         <v>0.7159959600333237</v>
@@ -8691,18 +8131,8 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA70" t="inlineStr">
-        <is>
-          <t>G5VbFe-2</t>
-        </is>
-      </c>
-      <c r="AB70" t="inlineStr">
-        <is>
-          <t>G5V</t>
-        </is>
-      </c>
       <c r="AC70" t="n">
-        <v>1.197930374837999</v>
+        <v>1.197930374837997</v>
       </c>
       <c r="AD70" t="n">
         <v>12.31845137597027</v>
@@ -8929,16 +8359,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA72" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
-      <c r="AB72" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
       <c r="AC72" t="n">
         <v>1.223627125271365</v>
       </c>
@@ -9002,7 +8422,7 @@
         <v>1.466963109333895</v>
       </c>
       <c r="Q73" t="n">
-        <v>0.09177873625991576</v>
+        <v>0.09177873625991573</v>
       </c>
       <c r="R73" t="n">
         <v>1.232070702796847</v>
@@ -9043,18 +8463,8 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA73" t="inlineStr">
-        <is>
-          <t>G0V</t>
-        </is>
-      </c>
-      <c r="AB73" t="inlineStr">
-        <is>
-          <t>G0V</t>
-        </is>
-      </c>
       <c r="AC73" t="n">
-        <v>1.232068383131733</v>
+        <v>1.232068383131732</v>
       </c>
       <c r="AD73" t="n">
         <v>14.01680510641773</v>
@@ -9154,16 +8564,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA74" t="inlineStr">
-        <is>
-          <t>G6V</t>
-        </is>
-      </c>
-      <c r="AB74" t="inlineStr">
-        <is>
-          <t>G6V</t>
-        </is>
-      </c>
       <c r="AC74" t="n">
         <v>1.2342497422876</v>
       </c>
@@ -9273,16 +8673,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA75" t="inlineStr">
-        <is>
-          <t>G2Va</t>
-        </is>
-      </c>
-      <c r="AB75" t="inlineStr">
-        <is>
-          <t>G2V</t>
-        </is>
-      </c>
       <c r="AC75" t="n">
         <v>1.237670106674188</v>
       </c>
@@ -9392,16 +8782,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA76" t="inlineStr">
-        <is>
-          <t>F9V</t>
-        </is>
-      </c>
-      <c r="AB76" t="inlineStr">
-        <is>
-          <t>F9V</t>
-        </is>
-      </c>
       <c r="AC76" t="n">
         <v>1.238251857708608</v>
       </c>
@@ -9511,16 +8891,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA77" t="inlineStr">
-        <is>
-          <t>G2-V</t>
-        </is>
-      </c>
-      <c r="AB77" t="inlineStr">
-        <is>
-          <t>G2V</t>
-        </is>
-      </c>
       <c r="AC77" t="n">
         <v>1.244930575736043</v>
       </c>
@@ -9627,16 +8997,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA78" t="inlineStr">
-        <is>
-          <t>K2.5V</t>
-        </is>
-      </c>
-      <c r="AB78" t="inlineStr">
-        <is>
-          <t>K2.5V</t>
-        </is>
-      </c>
       <c r="AC78" t="n">
         <v>1.246684924050531</v>
       </c>
@@ -9746,16 +9106,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA79" t="inlineStr">
-        <is>
-          <t>K3V</t>
-        </is>
-      </c>
-      <c r="AB79" t="inlineStr">
-        <is>
-          <t>K3V</t>
-        </is>
-      </c>
       <c r="AC79" t="n">
         <v>1.255528586686926</v>
       </c>
@@ -9865,16 +9215,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA80" t="inlineStr">
-        <is>
-          <t>G2IV</t>
-        </is>
-      </c>
-      <c r="AB80" t="inlineStr">
-        <is>
-          <t>G2IV</t>
-        </is>
-      </c>
       <c r="AC80" t="n">
         <v>1.265309102785178</v>
       </c>
@@ -9984,16 +9324,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA81" t="inlineStr">
-        <is>
-          <t>G6V</t>
-        </is>
-      </c>
-      <c r="AB81" t="inlineStr">
-        <is>
-          <t>G6V</t>
-        </is>
-      </c>
       <c r="AC81" t="n">
         <v>1.269365170048064</v>
       </c>
@@ -10103,16 +9433,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA82" t="inlineStr">
-        <is>
-          <t>M0V</t>
-        </is>
-      </c>
-      <c r="AB82" t="inlineStr">
-        <is>
-          <t>M0V</t>
-        </is>
-      </c>
       <c r="AC82" t="n">
         <v>1.281665990186646</v>
       </c>
@@ -10333,16 +9653,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA84" t="inlineStr">
-        <is>
-          <t>K2.5Vk:</t>
-        </is>
-      </c>
-      <c r="AB84" t="inlineStr">
-        <is>
-          <t>K2.5V</t>
-        </is>
-      </c>
       <c r="AC84" t="n">
         <v>1.288249204737161</v>
       </c>
@@ -10452,16 +9762,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA85" t="inlineStr">
-        <is>
-          <t>K0V</t>
-        </is>
-      </c>
-      <c r="AB85" t="inlineStr">
-        <is>
-          <t>K0V</t>
-        </is>
-      </c>
       <c r="AC85" t="n">
         <v>1.293009722301958</v>
       </c>
@@ -10571,16 +9871,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA86" t="inlineStr">
-        <is>
-          <t>K2.5Vk:</t>
-        </is>
-      </c>
-      <c r="AB86" t="inlineStr">
-        <is>
-          <t>K2.5V</t>
-        </is>
-      </c>
       <c r="AC86" t="n">
         <v>1.306871258457764</v>
       </c>
@@ -10685,16 +9975,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA87" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
-      <c r="AB87" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
       <c r="AC87" t="n">
         <v>1.308840066962156</v>
       </c>
@@ -10804,16 +10084,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA88" t="inlineStr">
-        <is>
-          <t>K4/5V</t>
-        </is>
-      </c>
-      <c r="AB88" t="inlineStr">
-        <is>
-          <t>K4/5V</t>
-        </is>
-      </c>
       <c r="AC88" t="n">
         <v>1.309857180926842</v>
       </c>
@@ -10885,7 +10155,7 @@
         <v>0.1056122764309012</v>
       </c>
       <c r="R89" t="n">
-        <v>1.315597361564893</v>
+        <v>1.315597361564894</v>
       </c>
       <c r="S89" t="n">
         <v>1.185166893634851</v>
@@ -10916,16 +10186,6 @@
       <c r="Z89" t="inlineStr">
         <is>
           <t>GAIA</t>
-        </is>
-      </c>
-      <c r="AA89" t="inlineStr">
-        <is>
-          <t>G2.5V</t>
-        </is>
-      </c>
-      <c r="AB89" t="inlineStr">
-        <is>
-          <t>G2.5V</t>
         </is>
       </c>
       <c r="AC89" t="n">
@@ -11037,16 +10297,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA90" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
-      <c r="AB90" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
       <c r="AC90" t="n">
         <v>1.316193876733624</v>
       </c>
@@ -11156,16 +10406,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA91" t="inlineStr">
-        <is>
-          <t>K3V</t>
-        </is>
-      </c>
-      <c r="AB91" t="inlineStr">
-        <is>
-          <t>K3V</t>
-        </is>
-      </c>
       <c r="AC91" t="n">
         <v>1.31888718860156</v>
       </c>
@@ -11201,7 +10441,7 @@
         <v>-56.44366680941792</v>
       </c>
       <c r="F92" t="n">
-        <v>7.078011894307138</v>
+        <v>7.078011894307137</v>
       </c>
       <c r="G92" t="n">
         <v>6.866890907287598</v>
@@ -11234,10 +10474,10 @@
         <v>0.8075752876774311</v>
       </c>
       <c r="Q92" t="n">
-        <v>0.1467204175415847</v>
+        <v>0.1467204175415846</v>
       </c>
       <c r="R92" t="n">
-        <v>1.333274305644923</v>
+        <v>1.333274305644922</v>
       </c>
       <c r="S92" t="n">
         <v>1.848206256583958</v>
@@ -11275,18 +10515,8 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA92" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
-      <c r="AB92" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
       <c r="AC92" t="n">
-        <v>1.333271042125484</v>
+        <v>1.333271042125483</v>
       </c>
       <c r="AD92" t="n">
         <v>14.82647987202467</v>
@@ -11394,16 +10624,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA93" t="inlineStr">
-        <is>
-          <t>G7IV</t>
-        </is>
-      </c>
-      <c r="AB93" t="inlineStr">
-        <is>
-          <t>G7IV</t>
-        </is>
-      </c>
       <c r="AC93" t="n">
         <v>1.345364616191713</v>
       </c>
@@ -11513,16 +10733,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA94" t="inlineStr">
-        <is>
-          <t>K5V</t>
-        </is>
-      </c>
-      <c r="AB94" t="inlineStr">
-        <is>
-          <t>K5V</t>
-        </is>
-      </c>
       <c r="AC94" t="n">
         <v>1.345620501735711</v>
       </c>
@@ -11632,16 +10842,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA95" t="inlineStr">
-        <is>
-          <t>G9V</t>
-        </is>
-      </c>
-      <c r="AB95" t="inlineStr">
-        <is>
-          <t>G9V</t>
-        </is>
-      </c>
       <c r="AC95" t="n">
         <v>1.346661409840882</v>
       </c>
@@ -11826,10 +11026,10 @@
         <v>1.860880880314579</v>
       </c>
       <c r="Q97" t="n">
-        <v>0.08311768856772306</v>
+        <v>0.08311768856772309</v>
       </c>
       <c r="R97" t="n">
-        <v>1.357087888634181</v>
+        <v>1.357087888634182</v>
       </c>
       <c r="S97" t="n">
         <v>0.6267989512448702</v>
@@ -11865,16 +11065,6 @@
       <c r="Z97" t="inlineStr">
         <is>
           <t>GAIA</t>
-        </is>
-      </c>
-      <c r="AA97" t="inlineStr">
-        <is>
-          <t>F9VFe+0.4</t>
-        </is>
-      </c>
-      <c r="AB97" t="inlineStr">
-        <is>
-          <t>F9V</t>
         </is>
       </c>
       <c r="AC97" t="n">
@@ -11983,16 +11173,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA98" t="inlineStr">
-        <is>
-          <t>G7.5IV-V</t>
-        </is>
-      </c>
-      <c r="AB98" t="inlineStr">
-        <is>
-          <t>G7.5IV-V</t>
-        </is>
-      </c>
       <c r="AC98" t="n">
         <v>1.357744852917667</v>
       </c>
@@ -12218,16 +11398,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA100" t="inlineStr">
-        <is>
-          <t>G1.5V</t>
-        </is>
-      </c>
-      <c r="AB100" t="inlineStr">
-        <is>
-          <t>G1.5V</t>
-        </is>
-      </c>
       <c r="AC100" t="n">
         <v>1.362513145042043</v>
       </c>
@@ -12337,16 +11507,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA101" t="inlineStr">
-        <is>
-          <t>K0.5V</t>
-        </is>
-      </c>
-      <c r="AB101" t="inlineStr">
-        <is>
-          <t>K0.5V</t>
-        </is>
-      </c>
       <c r="AC101" t="n">
         <v>1.362907393774444</v>
       </c>
@@ -12453,16 +11613,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA102" t="inlineStr">
-        <is>
-          <t>K3VFe-1.7</t>
-        </is>
-      </c>
-      <c r="AB102" t="inlineStr">
-        <is>
-          <t>K3V</t>
-        </is>
-      </c>
       <c r="AC102" t="n">
         <v>1.383070924943398</v>
       </c>
@@ -12683,16 +11833,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA104" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
-      <c r="AB104" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
       <c r="AC104" t="n">
         <v>1.392138947636566</v>
       </c>
@@ -12802,16 +11942,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA105" t="inlineStr">
-        <is>
-          <t>G3V</t>
-        </is>
-      </c>
-      <c r="AB105" t="inlineStr">
-        <is>
-          <t>G3V</t>
-        </is>
-      </c>
       <c r="AC105" t="n">
         <v>1.393289447770247</v>
       </c>
@@ -12921,16 +12051,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA106" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
-      <c r="AB106" t="inlineStr">
-        <is>
-          <t>K1V</t>
-        </is>
-      </c>
       <c r="AC106" t="n">
         <v>1.395205962521868</v>
       </c>
@@ -13154,16 +12274,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA108" t="inlineStr">
-        <is>
-          <t>G2V</t>
-        </is>
-      </c>
-      <c r="AB108" t="inlineStr">
-        <is>
-          <t>G2V</t>
-        </is>
-      </c>
       <c r="AC108" t="n">
         <v>1.412445050981794</v>
       </c>
@@ -13273,16 +12383,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA109" t="inlineStr">
-        <is>
-          <t>G9V</t>
-        </is>
-      </c>
-      <c r="AB109" t="inlineStr">
-        <is>
-          <t>G9V</t>
-        </is>
-      </c>
       <c r="AC109" t="n">
         <v>1.412839535836644</v>
       </c>
@@ -13387,16 +12487,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA110" t="inlineStr">
-        <is>
-          <t>K7-V(k)</t>
-        </is>
-      </c>
-      <c r="AB110" t="inlineStr">
-        <is>
-          <t>K7V</t>
-        </is>
-      </c>
       <c r="AC110" t="n">
         <v>1.414583634984824</v>
       </c>
@@ -13506,16 +12596,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA111" t="inlineStr">
-        <is>
-          <t>K4.5Vk:</t>
-        </is>
-      </c>
-      <c r="AB111" t="inlineStr">
-        <is>
-          <t>K4.5V</t>
-        </is>
-      </c>
       <c r="AC111" t="n">
         <v>1.416810917432006</v>
       </c>
@@ -13625,21 +12705,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA112" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
-      <c r="AB112" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
       <c r="AC112" t="n">
         <v>1.419464368419534</v>
       </c>
       <c r="AD112" t="n">
-        <v>16.16961333282446</v>
+        <v>16.16961333282445</v>
       </c>
       <c r="AE112" t="inlineStr">
         <is>
@@ -13860,16 +12930,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA114" t="inlineStr">
-        <is>
-          <t>G2V</t>
-        </is>
-      </c>
-      <c r="AB114" t="inlineStr">
-        <is>
-          <t>G2V</t>
-        </is>
-      </c>
       <c r="AC114" t="n">
         <v>1.420482012828254</v>
       </c>
@@ -14090,16 +13150,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA116" t="inlineStr">
-        <is>
-          <t>K3V</t>
-        </is>
-      </c>
-      <c r="AB116" t="inlineStr">
-        <is>
-          <t>K3V</t>
-        </is>
-      </c>
       <c r="AC116" t="n">
         <v>1.424545578856465</v>
       </c>
@@ -14209,16 +13259,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA117" t="inlineStr">
-        <is>
-          <t>M0.5V</t>
-        </is>
-      </c>
-      <c r="AB117" t="inlineStr">
-        <is>
-          <t>M0.5V</t>
-        </is>
-      </c>
       <c r="AC117" t="n">
         <v>1.426086891702461</v>
       </c>
@@ -14334,7 +13374,7 @@
         <v>1.427090630932611</v>
       </c>
       <c r="AD118" t="n">
-        <v>43.71816825476425</v>
+        <v>43.71816825476424</v>
       </c>
       <c r="AE118" t="inlineStr">
         <is>
@@ -14439,16 +13479,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA119" t="inlineStr">
-        <is>
-          <t>G2IV-V</t>
-        </is>
-      </c>
-      <c r="AB119" t="inlineStr">
-        <is>
-          <t>G2IV-V</t>
-        </is>
-      </c>
       <c r="AC119" t="n">
         <v>1.429153105927285</v>
       </c>
@@ -14674,16 +13704,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA121" t="inlineStr">
-        <is>
-          <t>G9IV-V</t>
-        </is>
-      </c>
-      <c r="AB121" t="inlineStr">
-        <is>
-          <t>G9IV-V</t>
-        </is>
-      </c>
       <c r="AC121" t="n">
         <v>1.432236243622335</v>
       </c>
@@ -14904,16 +13924,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA123" t="inlineStr">
-        <is>
-          <t>G0IV</t>
-        </is>
-      </c>
-      <c r="AB123" t="inlineStr">
-        <is>
-          <t>G0IV</t>
-        </is>
-      </c>
       <c r="AC123" t="n">
         <v>1.457058359037807</v>
       </c>
@@ -15065,7 +14075,7 @@
         <v>0.7957516031522688</v>
       </c>
       <c r="F125" t="n">
-        <v>6.895888036379815</v>
+        <v>6.895888036379814</v>
       </c>
       <c r="G125" t="n">
         <v>6.703805923461914</v>
@@ -15098,10 +14108,10 @@
         <v>0.8939739511304585</v>
       </c>
       <c r="Q125" t="n">
-        <v>0.1490097064217218</v>
+        <v>0.1490097064217217</v>
       </c>
       <c r="R125" t="n">
-        <v>1.466649177966211</v>
+        <v>1.46664917796621</v>
       </c>
       <c r="S125" t="n">
         <v>1.742480332590559</v>
@@ -15134,18 +14144,8 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA125" t="inlineStr">
-        <is>
-          <t>K0V</t>
-        </is>
-      </c>
-      <c r="AB125" t="inlineStr">
-        <is>
-          <t>K0V</t>
-        </is>
-      </c>
       <c r="AC125" t="n">
-        <v>1.466645451681133</v>
+        <v>1.466645451681132</v>
       </c>
       <c r="AD125" t="n">
         <v>15.81931741178505</v>
@@ -15253,16 +14253,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA126" t="inlineStr">
-        <is>
-          <t>G8V</t>
-        </is>
-      </c>
-      <c r="AB126" t="inlineStr">
-        <is>
-          <t>G8V</t>
-        </is>
-      </c>
       <c r="AC126" t="n">
         <v>1.475847044306138</v>
       </c>
@@ -15372,16 +14362,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA127" t="inlineStr">
-        <is>
-          <t>G9V</t>
-        </is>
-      </c>
-      <c r="AB127" t="inlineStr">
-        <is>
-          <t>G9V</t>
-        </is>
-      </c>
       <c r="AC127" t="n">
         <v>1.481576761467434</v>
       </c>
@@ -15483,21 +14463,11 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA128" t="inlineStr">
-        <is>
-          <t>G6V</t>
-        </is>
-      </c>
-      <c r="AB128" t="inlineStr">
-        <is>
-          <t>G6V</t>
-        </is>
-      </c>
       <c r="AC128" t="n">
         <v>1.483366132894098</v>
       </c>
       <c r="AD128" t="n">
-        <v>16.95317213092453</v>
+        <v>16.95317213092454</v>
       </c>
       <c r="AE128" t="inlineStr">
         <is>
@@ -15602,16 +14572,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA129" t="inlineStr">
-        <is>
-          <t>G6.5V</t>
-        </is>
-      </c>
-      <c r="AB129" t="inlineStr">
-        <is>
-          <t>G6.5V</t>
-        </is>
-      </c>
       <c r="AC129" t="n">
         <v>1.494642602191986</v>
       </c>
@@ -15721,16 +14681,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA130" t="inlineStr">
-        <is>
-          <t>K2Vk:</t>
-        </is>
-      </c>
-      <c r="AB130" t="inlineStr">
-        <is>
-          <t>K2V</t>
-        </is>
-      </c>
       <c r="AC130" t="n">
         <v>1.496376602428396</v>
       </c>
@@ -15840,16 +14790,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA131" t="inlineStr">
-        <is>
-          <t>G0V</t>
-        </is>
-      </c>
-      <c r="AB131" t="inlineStr">
-        <is>
-          <t>G0V</t>
-        </is>
-      </c>
       <c r="AC131" t="n">
         <v>1.4976843859931</v>
       </c>
@@ -15954,16 +14894,6 @@
           <t>GAIA</t>
         </is>
       </c>
-      <c r="AA132" t="inlineStr">
-        <is>
-          <t>K0</t>
-        </is>
-      </c>
-      <c r="AB132" t="inlineStr">
-        <is>
-          <t>K0</t>
-        </is>
-      </c>
       <c r="AC132" t="n">
         <v>1.497859894483765</v>
       </c>
@@ -16071,16 +15001,6 @@
       <c r="Z133" t="inlineStr">
         <is>
           <t>GAIA</t>
-        </is>
-      </c>
-      <c r="AA133" t="inlineStr">
-        <is>
-          <t>K0V</t>
-        </is>
-      </c>
-      <c r="AB133" t="inlineStr">
-        <is>
-          <t>K0V</t>
         </is>
       </c>
       <c r="AC133" t="n">

</xml_diff>